<commit_message>
Added parent career analyses and school location analyses to summary
</commit_message>
<xml_diff>
--- a/Initial demographics summary.xlsx
+++ b/Initial demographics summary.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12792" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Julian analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="More Analyses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>PVSCIE</t>
   </si>
@@ -595,25 +595,43 @@
     <t>Non-sci</t>
   </si>
   <si>
-    <t>Sci</t>
-  </si>
-  <si>
     <t>mother %</t>
   </si>
   <si>
-    <t>mother score</t>
-  </si>
-  <si>
     <t>father %</t>
   </si>
   <si>
-    <t>father score</t>
-  </si>
-  <si>
-    <t>student %</t>
-  </si>
-  <si>
-    <t>student score</t>
+    <t>Sci, medical</t>
+  </si>
+  <si>
+    <t>Sci, engineer/tech</t>
+  </si>
+  <si>
+    <t>urban %</t>
+  </si>
+  <si>
+    <t>not-urban %</t>
+  </si>
+  <si>
+    <t>urban</t>
+  </si>
+  <si>
+    <t>not urban</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>self %</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>father</t>
+  </si>
+  <si>
+    <t>mother</t>
   </si>
 </sst>
 </file>
@@ -1219,29 +1237,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1309,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1344,7 +1362,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1415,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1468,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>27</v>
@@ -1462,7 +1480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1496,7 +1514,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1513,7 +1531,7 @@
         <v>16.200000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1548,7 @@
         <v>24.100000000000009</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1547,7 +1565,7 @@
         <v>6.7000000000000028</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>11</v>
       </c>
@@ -1564,7 +1582,7 @@
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
@@ -1581,7 +1599,7 @@
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
     </row>
-    <row r="15" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>17</v>
       </c>
@@ -1598,7 +1616,7 @@
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>21</v>
       </c>
@@ -1615,7 +1633,7 @@
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
     </row>
-    <row r="17" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>39</v>
       </c>
@@ -1632,7 +1650,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>22</v>
       </c>
@@ -1649,7 +1667,7 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>23</v>
       </c>
@@ -1666,7 +1684,7 @@
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>24</v>
       </c>
@@ -1683,7 +1701,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>25</v>
       </c>
@@ -1700,7 +1718,7 @@
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>26</v>
       </c>
@@ -1717,7 +1735,7 @@
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
     </row>
-    <row r="23" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>18</v>
       </c>
@@ -1734,7 +1752,7 @@
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
     </row>
-    <row r="24" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
@@ -1751,7 +1769,7 @@
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>20</v>
       </c>
@@ -1768,37 +1786,37 @@
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1826,83 +1844,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2">
+        <v>498.95</v>
+      </c>
+      <c r="C2">
         <v>87.87</v>
       </c>
-      <c r="C2">
-        <v>498.95</v>
-      </c>
       <c r="D2">
-        <v>93.64</v>
+        <v>497.66</v>
       </c>
       <c r="E2">
-        <v>497.66</v>
+        <v>90.34</v>
       </c>
       <c r="F2">
+        <v>487.76</v>
+      </c>
+      <c r="G2">
         <v>59.89</v>
       </c>
-      <c r="G2">
-        <v>487.76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B3">
-        <v>12.13</v>
+        <v>570.16999999999996</v>
       </c>
       <c r="C3">
-        <v>513.63</v>
+        <v>1.38</v>
       </c>
       <c r="D3">
-        <v>9.66</v>
+        <v>554.24</v>
       </c>
       <c r="E3">
-        <v>550.70000000000005</v>
+        <v>7.3</v>
       </c>
       <c r="F3">
-        <v>40.11</v>
+        <v>543.75</v>
       </c>
       <c r="G3">
-        <v>516.28</v>
+        <v>16.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>506.39</v>
+      </c>
+      <c r="C4">
+        <v>10.75</v>
+      </c>
+      <c r="D4">
+        <v>539.75</v>
+      </c>
+      <c r="E4">
+        <v>2.36</v>
+      </c>
+      <c r="F4">
+        <v>296.83</v>
+      </c>
+      <c r="G4">
+        <v>23.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>497.45</v>
+      </c>
+      <c r="C7">
+        <v>472.61</v>
+      </c>
+      <c r="D7">
+        <v>60.98</v>
+      </c>
+      <c r="E7">
+        <v>39.020000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>552.86</v>
+      </c>
+      <c r="C8">
+        <v>530.66999999999996</v>
+      </c>
+      <c r="D8">
+        <v>58.95</v>
+      </c>
+      <c r="E8">
+        <v>41.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>503.99</v>
+      </c>
+      <c r="C9">
+        <v>484.06</v>
+      </c>
+      <c r="D9">
+        <v>64.08</v>
+      </c>
+      <c r="E9">
+        <v>35.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>